<commit_message>
Fixed last bug (hopefully)
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Win ratios</t>
   </si>
@@ -56,22 +56,53 @@
     <t>44/6</t>
   </si>
   <si>
-    <t>35/15</t>
-  </si>
-  <si>
-    <t>33/17</t>
-  </si>
-  <si>
     <t>22/28</t>
+  </si>
+  <si>
+    <t>Heuristic 1</t>
+  </si>
+  <si>
+    <t>Heuristic 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -86,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -94,13 +125,252 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,157 +651,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:J18"/>
+  <dimension ref="C1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I2" sqref="I2:O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" customWidth="1"/>
+    <col min="10" max="15" width="6.7109375" style="3" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="3:15" ht="24" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="3:15" ht="27" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
-      <c r="D2" s="1">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="22"/>
+    </row>
+    <row r="3" spans="3:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E3" s="1">
         <v>2</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F3" s="1">
         <v>3</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G3" s="1">
         <v>4</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H3" s="1">
         <v>5</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="1">
+      <c r="I3" s="1"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="13">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="L3" s="14">
+        <v>2</v>
+      </c>
+      <c r="M3" s="14">
+        <v>3</v>
+      </c>
+      <c r="N3" s="14">
+        <v>4</v>
+      </c>
+      <c r="O3" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="23">
+        <v>1</v>
+      </c>
+      <c r="K4" s="10">
+        <v>50</v>
+      </c>
+      <c r="L4" s="11">
+        <v>0</v>
+      </c>
+      <c r="M4" s="11">
+        <v>14</v>
+      </c>
+      <c r="N4" s="11">
+        <v>0</v>
+      </c>
+      <c r="O4" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="18"/>
+      <c r="J5" s="23">
+        <v>2</v>
+      </c>
+      <c r="K5" s="8">
+        <v>100</v>
+      </c>
+      <c r="L5" s="4">
+        <v>54</v>
+      </c>
+      <c r="M5" s="4">
+        <v>78</v>
+      </c>
+      <c r="N5" s="4">
+        <v>52</v>
+      </c>
+      <c r="O5" s="5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="18"/>
+      <c r="J6" s="23">
+        <v>3</v>
+      </c>
+      <c r="K6" s="8">
+        <v>86</v>
+      </c>
+      <c r="L6" s="4">
+        <v>22</v>
+      </c>
+      <c r="M6" s="4">
+        <v>48</v>
+      </c>
+      <c r="N6" s="4">
+        <v>22</v>
+      </c>
+      <c r="O6" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C7" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="18"/>
+      <c r="J7" s="23">
+        <v>4</v>
+      </c>
+      <c r="K7" s="8">
+        <v>100</v>
+      </c>
+      <c r="L7" s="4">
+        <v>48</v>
+      </c>
+      <c r="M7" s="4">
+        <v>78</v>
+      </c>
+      <c r="N7" s="4">
+        <v>44</v>
+      </c>
+      <c r="O7" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="19"/>
+      <c r="J8" s="24">
+        <v>5</v>
+      </c>
+      <c r="K8" s="9">
+        <v>100</v>
+      </c>
+      <c r="L8" s="6">
+        <v>58</v>
+      </c>
+      <c r="M8" s="6">
+        <v>88</v>
+      </c>
+      <c r="N8" s="6">
+        <v>44</v>
+      </c>
+      <c r="O8" s="7">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I9" s="1"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -539,9 +915,10 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -549,9 +926,10 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -559,9 +937,10 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -569,9 +948,10 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -579,9 +959,10 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -589,9 +970,10 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -599,9 +981,10 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -609,9 +992,10 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -619,9 +1003,37 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="I4:I8"/>
+  </mergeCells>
+  <conditionalFormatting sqref="K4:O8">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>